<commit_message>
Add Driver column to Trip report template
</commit_message>
<xml_diff>
--- a/templates/export/trips.xlsx
+++ b/templates/export/trips.xlsx
@@ -34,7 +34,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>jx:area(lastCell="I9")</t>
+          <t>jx:area(lastCell="J9")</t>
         </r>
       </text>
     </comment>
@@ -48,7 +48,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t xml:space="preserve">jx:each(items="devices", var="device", lastCell="I9" multisheet="sheetNames")
+          <t xml:space="preserve">jx:each(items="devices", var="device", lastCell="J9" multisheet="sheetNames")
 </t>
         </r>
       </text>
@@ -63,7 +63,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>jx:each(items="device.objects", var="trip", lastCell="I9")</t>
+          <t>jx:each(items="device.objects", var="trip", lastCell="J9")</t>
         </r>
       </text>
     </comment>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Report type:</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", trip.endTime, locale, timezone)}</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>${trip.driverName ? trip.driverName : trip.driverUniqueId}</t>
   </si>
 </sst>
 </file>
@@ -826,7 +832,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -843,10 +849,11 @@
     <col min="7" max="7" width="13.85546875"/>
     <col min="8" max="8" width="15.85546875"/>
     <col min="9" max="9" width="14.42578125"/>
-    <col min="10" max="1025" width="8.7109375"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -857,7 +864,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -872,7 +879,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="5"/>
       <c r="C3" s="3"/>
@@ -883,7 +890,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -898,7 +905,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -913,7 +920,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -928,7 +935,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="3"/>
@@ -939,7 +946,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -967,8 +974,11 @@
       <c r="I8" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>24</v>
       </c>
@@ -996,8 +1006,11 @@
       <c r="I9" s="13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1008,7 +1021,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
       <c r="C11" s="3"/>
@@ -1019,7 +1032,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="16"/>
       <c r="C12" s="3"/>
@@ -1030,7 +1043,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
       <c r="C13" s="3"/>
@@ -1041,7 +1054,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="3"/>
@@ -1052,7 +1065,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="18"/>
       <c r="C15" s="3"/>

</xml_diff>